<commit_message>
validation of UFA, energy, carbon
</commit_message>
<xml_diff>
--- a/Data/model_outputs_baseline/UFA/carbon_emissions_AB_df.xlsx
+++ b/Data/model_outputs_baseline/UFA/carbon_emissions_AB_df.xlsx
@@ -2851,7 +2851,7 @@
         <v>301</v>
       </c>
       <c r="B303" t="n">
-        <v>11983600.40858057</v>
+        <v>6590961.680234829</v>
       </c>
     </row>
     <row r="304">
@@ -2859,7 +2859,7 @@
         <v>302</v>
       </c>
       <c r="B304" t="n">
-        <v>24109499.24552681</v>
+        <v>13260313.41987303</v>
       </c>
     </row>
     <row r="305">
@@ -2867,7 +2867,7 @@
         <v>303</v>
       </c>
       <c r="B305" t="n">
-        <v>36385240.74239202</v>
+        <v>20012049.74384139</v>
       </c>
     </row>
     <row r="306">
@@ -2875,7 +2875,7 @@
         <v>304</v>
       </c>
       <c r="B306" t="n">
-        <v>48811083.22630218</v>
+        <v>26846390.80162627</v>
       </c>
     </row>
     <row r="307">
@@ -2883,7 +2883,7 @@
         <v>305</v>
       </c>
       <c r="B307" t="n">
-        <v>61389405.94803565</v>
+        <v>33764575.78841169</v>
       </c>
     </row>
     <row r="308">
@@ -2891,7 +2891,7 @@
         <v>306</v>
       </c>
       <c r="B308" t="n">
-        <v>74123088.03592029</v>
+        <v>40768448.02628388</v>
       </c>
     </row>
     <row r="309">
@@ -2899,7 +2899,7 @@
         <v>307</v>
       </c>
       <c r="B309" t="n">
-        <v>87014375.78095023</v>
+        <v>47858707.60929731</v>
       </c>
     </row>
     <row r="310">
@@ -2907,7 +2907,7 @@
         <v>308</v>
       </c>
       <c r="B310" t="n">
-        <v>100066676.7130346</v>
+        <v>55037684.35121018</v>
       </c>
     </row>
     <row r="311">
@@ -2915,7 +2915,7 @@
         <v>309</v>
       </c>
       <c r="B311" t="n">
-        <v>113281744.0853664</v>
+        <v>62306219.63732316</v>
       </c>
     </row>
     <row r="312">
@@ -2923,7 +2923,7 @@
         <v>310</v>
       </c>
       <c r="B312" t="n">
-        <v>126662959.383555</v>
+        <v>69666197.16867729</v>
       </c>
     </row>
     <row r="313">
@@ -2931,7 +2931,7 @@
         <v>311</v>
       </c>
       <c r="B313" t="n">
-        <v>140212550.7232948</v>
+        <v>77118677.83913752</v>
       </c>
     </row>
     <row r="314">
@@ -2939,7 +2939,7 @@
         <v>312</v>
       </c>
       <c r="B314" t="n">
-        <v>153933252.6521844</v>
+        <v>84665449.48949195</v>
       </c>
     </row>
     <row r="315">
@@ -2947,7 +2947,7 @@
         <v>313</v>
       </c>
       <c r="B315" t="n">
-        <v>167827875.1414022</v>
+        <v>92307787.66886139</v>
       </c>
     </row>
     <row r="316">
@@ -2955,7 +2955,7 @@
         <v>314</v>
       </c>
       <c r="B316" t="n">
-        <v>181898939.5941035</v>
+        <v>100047035.7618821</v>
       </c>
     </row>
     <row r="317">
@@ -2963,7 +2963,7 @@
         <v>315</v>
       </c>
       <c r="B317" t="n">
-        <v>196148841.3668919</v>
+        <v>107885098.2150885</v>
       </c>
     </row>
     <row r="318">
@@ -2971,7 +2971,7 @@
         <v>316</v>
       </c>
       <c r="B318" t="n">
-        <v>210580676.7268349</v>
+        <v>115822841.8591289</v>
       </c>
     </row>
     <row r="319">
@@ -2979,7 +2979,7 @@
         <v>317</v>
       </c>
       <c r="B319" t="n">
-        <v>225196740.6073617</v>
+        <v>123862520.2881881</v>
       </c>
     </row>
     <row r="320">
@@ -2987,7 +2987,7 @@
         <v>318</v>
       </c>
       <c r="B320" t="n">
-        <v>240000036.1786282</v>
+        <v>132004395.7479948</v>
       </c>
     </row>
     <row r="321">
@@ -2995,7 +2995,7 @@
         <v>319</v>
       </c>
       <c r="B321" t="n">
-        <v>254992338.7524262</v>
+        <v>140251109.8047367</v>
       </c>
     </row>
     <row r="322">
@@ -3003,7 +3003,7 @@
         <v>320</v>
       </c>
       <c r="B322" t="n">
-        <v>270177256.3732307</v>
+        <v>148602923.5460071</v>
       </c>
     </row>
     <row r="323">
@@ -3011,7 +3011,7 @@
         <v>321</v>
       </c>
       <c r="B323" t="n">
-        <v>285556833.5977859</v>
+        <v>157062355.9572497</v>
       </c>
     </row>
     <row r="324">
@@ -3019,7 +3019,7 @@
         <v>322</v>
       </c>
       <c r="B324" t="n">
-        <v>301133497.876685</v>
+        <v>165630286.2139201</v>
       </c>
     </row>
     <row r="325">
@@ -3027,7 +3027,7 @@
         <v>323</v>
       </c>
       <c r="B325" t="n">
-        <v>316910073.7869202</v>
+        <v>174307864.0912819</v>
       </c>
     </row>
     <row r="326">
@@ -3035,7 +3035,7 @@
         <v>324</v>
       </c>
       <c r="B326" t="n">
-        <v>332888704.1142461</v>
+        <v>183096704.5116616</v>
       </c>
     </row>
     <row r="327">
@@ -3043,7 +3043,7 @@
         <v>325</v>
       </c>
       <c r="B327" t="n">
-        <v>349072373.0651312</v>
+        <v>191998406.8697655</v>
       </c>
     </row>
     <row r="328">
@@ -3051,7 +3051,7 @@
         <v>326</v>
       </c>
       <c r="B328" t="n">
-        <v>365462746.8894116</v>
+        <v>201014014.5525599</v>
       </c>
     </row>
     <row r="329">
@@ -3059,7 +3059,7 @@
         <v>327</v>
       </c>
       <c r="B329" t="n">
-        <v>382062875.9694748</v>
+        <v>210144923.3290028</v>
       </c>
     </row>
     <row r="330">
@@ -3067,7 +3067,7 @@
         <v>328</v>
       </c>
       <c r="B330" t="n">
-        <v>398874825.7032524</v>
+        <v>219391900.7786142</v>
       </c>
     </row>
     <row r="331">
@@ -3075,7 +3075,7 @@
         <v>329</v>
       </c>
       <c r="B331" t="n">
-        <v>415900522.2335806</v>
+        <v>228756903.6538061</v>
       </c>
     </row>
     <row r="332">
@@ -3083,7 +3083,7 @@
         <v>330</v>
       </c>
       <c r="B332" t="n">
-        <v>433142630.9041706</v>
+        <v>238240840.0914784</v>
       </c>
     </row>
     <row r="333">
@@ -3091,7 +3091,7 @@
         <v>331</v>
       </c>
       <c r="B333" t="n">
-        <v>450603188.8640594</v>
+        <v>247845041.9717301</v>
       </c>
     </row>
     <row r="334">
@@ -3099,7 +3099,7 @@
         <v>332</v>
       </c>
       <c r="B334" t="n">
-        <v>468284073.4616466</v>
+        <v>257570412.9667169</v>
       </c>
     </row>
     <row r="335">
@@ -3107,7 +3107,7 @@
         <v>333</v>
       </c>
       <c r="B335" t="n">
-        <v>486187584.4480807</v>
+        <v>267418057.8525041</v>
       </c>
     </row>
     <row r="336">
@@ -3115,7 +3115,7 @@
         <v>334</v>
       </c>
       <c r="B336" t="n">
-        <v>504315531.6374006</v>
+        <v>277388958.96777</v>
       </c>
     </row>
     <row r="337">
@@ -3123,7 +3123,7 @@
         <v>335</v>
       </c>
       <c r="B337" t="n">
-        <v>522669695.9944144</v>
+        <v>287484944.0616337</v>
       </c>
     </row>
     <row r="338">
@@ -3131,7 +3131,7 @@
         <v>336</v>
       </c>
       <c r="B338" t="n">
-        <v>541252122.7816453</v>
+        <v>297706297.5889311</v>
       </c>
     </row>
     <row r="339">
@@ -3139,7 +3139,7 @@
         <v>337</v>
       </c>
       <c r="B339" t="n">
-        <v>560064301.142359</v>
+        <v>308054139.5575461</v>
       </c>
     </row>
     <row r="340">
@@ -3147,7 +3147,7 @@
         <v>338</v>
       </c>
       <c r="B340" t="n">
-        <v>579107792.2060256</v>
+        <v>318529141.3853505</v>
       </c>
     </row>
     <row r="341">
@@ -3155,7 +3155,7 @@
         <v>339</v>
       </c>
       <c r="B341" t="n">
-        <v>598384542.8456945</v>
+        <v>329132128.983069</v>
       </c>
     </row>
     <row r="342">
@@ -3163,7 +3163,7 @@
         <v>340</v>
       </c>
       <c r="B342" t="n">
-        <v>617895193.6290576</v>
+        <v>339864495.8470829</v>
       </c>
     </row>
     <row r="343">
@@ -3171,7 +3171,7 @@
         <v>341</v>
       </c>
       <c r="B343" t="n">
-        <v>637641639.5571072</v>
+        <v>350725929.1520851</v>
       </c>
     </row>
     <row r="344">
@@ -3179,7 +3179,7 @@
         <v>342</v>
       </c>
       <c r="B344" t="n">
-        <v>657624387.4790373</v>
+        <v>361717360.0314116</v>
       </c>
     </row>
     <row r="345">
@@ -3187,7 +3187,7 @@
         <v>343</v>
       </c>
       <c r="B345" t="n">
-        <v>677845303.7044461</v>
+        <v>372840124.3684502</v>
       </c>
     </row>
     <row r="346">
@@ -3195,7 +3195,7 @@
         <v>344</v>
       </c>
       <c r="B346" t="n">
-        <v>698304754.9861217</v>
+        <v>384093899.8100486</v>
       </c>
     </row>
     <row r="347">
@@ -3203,7 +3203,7 @@
         <v>345</v>
       </c>
       <c r="B347" t="n">
-        <v>719003158.3312334</v>
+        <v>395479114.0801693</v>
       </c>
     </row>
     <row r="348">
@@ -3211,7 +3211,7 @@
         <v>346</v>
       </c>
       <c r="B348" t="n">
-        <v>739942050.9946457</v>
+        <v>406996578.067414</v>
       </c>
     </row>
     <row r="349">
@@ -3219,7 +3219,7 @@
         <v>347</v>
       </c>
       <c r="B349" t="n">
-        <v>761121242.5934942</v>
+        <v>418646666.8436334</v>
       </c>
     </row>
     <row r="350">
@@ -3227,7 +3227,7 @@
         <v>348</v>
       </c>
       <c r="B350" t="n">
-        <v>782541330.4552808</v>
+        <v>430428844.7618352</v>
       </c>
     </row>
     <row r="351">
@@ -3235,7 +3235,7 @@
         <v>349</v>
       </c>
       <c r="B351" t="n">
-        <v>804202139.6493908</v>
+        <v>442343738.0189191</v>
       </c>
     </row>
     <row r="352">
@@ -3243,7 +3243,7 @@
         <v>350</v>
       </c>
       <c r="B352" t="n">
-        <v>826104397.1788691</v>
+        <v>454390909.7727851</v>
       </c>
     </row>
     <row r="353">
@@ -3251,7 +3251,7 @@
         <v>351</v>
       </c>
       <c r="B353" t="n">
-        <v>848247096.6515927</v>
+        <v>466570211.3994031</v>
       </c>
     </row>
     <row r="354">
@@ -3259,7 +3259,7 @@
         <v>352</v>
       </c>
       <c r="B354" t="n">
-        <v>870630689.0828905</v>
+        <v>478882417.8001597</v>
       </c>
     </row>
     <row r="355">
@@ -3267,7 +3267,7 @@
         <v>353</v>
       </c>
       <c r="B355" t="n">
-        <v>893254134.1860774</v>
+        <v>491326206.7242696</v>
       </c>
     </row>
     <row r="356">
@@ -3275,7 +3275,7 @@
         <v>354</v>
       </c>
       <c r="B356" t="n">
-        <v>916116999.6715529</v>
+        <v>503902384.0998814</v>
       </c>
     </row>
     <row r="357">
@@ -3283,7 +3283,7 @@
         <v>355</v>
       </c>
       <c r="B357" t="n">
-        <v>939218091.7780775</v>
+        <v>516609661.0542123</v>
       </c>
     </row>
     <row r="358">
@@ -3291,7 +3291,7 @@
         <v>356</v>
       </c>
       <c r="B358" t="n">
-        <v>962428420.5297517</v>
+        <v>529376633.4242564</v>
       </c>
     </row>
     <row r="359">
@@ -3299,7 +3299,7 @@
         <v>357</v>
       </c>
       <c r="B359" t="n">
-        <v>985873093.9075214</v>
+        <v>542272635.1884423</v>
       </c>
     </row>
     <row r="360">
@@ -3307,7 +3307,7 @@
         <v>358</v>
       </c>
       <c r="B360" t="n">
-        <v>1009551360.54368</v>
+        <v>555297030.7867391</v>
       </c>
     </row>
     <row r="361">
@@ -3315,7 +3315,7 @@
         <v>359</v>
       </c>
       <c r="B361" t="n">
-        <v>1033461190.850898</v>
+        <v>568449032.3538011</v>
       </c>
     </row>
     <row r="362">
@@ -3323,7 +3323,7 @@
         <v>360</v>
       </c>
       <c r="B362" t="n">
-        <v>1057601172.63974</v>
+        <v>581727443.4090292</v>
       </c>
     </row>
     <row r="363">
@@ -3331,7 +3331,7 @@
         <v>361</v>
       </c>
       <c r="B363" t="n">
-        <v>1081968964.4237</v>
+        <v>595131434.5082816</v>
       </c>
     </row>
     <row r="364">
@@ -3339,7 +3339,7 @@
         <v>362</v>
       </c>
       <c r="B364" t="n">
-        <v>1106562352.087063</v>
+        <v>608658823.4956042</v>
       </c>
     </row>
     <row r="365">
@@ -3347,7 +3347,7 @@
         <v>363</v>
       </c>
       <c r="B365" t="n">
-        <v>1131378578.620336</v>
+        <v>622309190.8419447</v>
       </c>
     </row>
     <row r="366">
@@ -3355,7 +3355,7 @@
         <v>364</v>
       </c>
       <c r="B366" t="n">
-        <v>1156415296.086895</v>
+        <v>636080231.7582297</v>
       </c>
     </row>
     <row r="367">
@@ -3363,7 +3363,7 @@
         <v>365</v>
       </c>
       <c r="B367" t="n">
-        <v>1181669283.883677</v>
+        <v>649971400.4613445</v>
       </c>
     </row>
     <row r="368">
@@ -3371,7 +3371,7 @@
         <v>366</v>
       </c>
       <c r="B368" t="n">
-        <v>1207137246.440516</v>
+        <v>663980657.322772</v>
       </c>
     </row>
     <row r="369">
@@ -3379,7 +3379,7 @@
         <v>367</v>
       </c>
       <c r="B369" t="n">
-        <v>1232816368.899849</v>
+        <v>678105817.5523417</v>
       </c>
     </row>
     <row r="370">
@@ -3387,7 +3387,7 @@
         <v>368</v>
       </c>
       <c r="B370" t="n">
-        <v>1258702594.797298</v>
+        <v>692345161.7187333</v>
       </c>
     </row>
     <row r="371">
@@ -3395,7 +3395,7 @@
         <v>369</v>
       </c>
       <c r="B371" t="n">
-        <v>1284792030.589759</v>
+        <v>706695610.2934171</v>
       </c>
     </row>
     <row r="372">
@@ -3403,7 +3403,7 @@
         <v>370</v>
       </c>
       <c r="B372" t="n">
-        <v>1311080961.415303</v>
+        <v>721156171.1563927</v>
       </c>
     </row>
     <row r="373">
@@ -3411,7 +3411,7 @@
         <v>371</v>
       </c>
       <c r="B373" t="n">
-        <v>1333102775.749794</v>
+        <v>733269591.7866001</v>
       </c>
     </row>
     <row r="374">
@@ -3419,7 +3419,7 @@
         <v>372</v>
       </c>
       <c r="B374" t="n">
-        <v>1355282352.104061</v>
+        <v>745469838.4593375</v>
       </c>
     </row>
     <row r="375">
@@ -3427,7 +3427,7 @@
         <v>373</v>
       </c>
       <c r="B375" t="n">
-        <v>1377614045.435207</v>
+        <v>757753611.0745714</v>
       </c>
     </row>
     <row r="376">
@@ -3435,7 +3435,7 @@
         <v>374</v>
       </c>
       <c r="B376" t="n">
-        <v>1400121480.823915</v>
+        <v>770132476.5362041</v>
       </c>
     </row>
     <row r="377">
@@ -3443,7 +3443,7 @@
         <v>375</v>
       </c>
       <c r="B377" t="n">
-        <v>1422772561.567305</v>
+        <v>782589912.0362105</v>
       </c>
     </row>
     <row r="378">
@@ -3451,7 +3451,7 @@
         <v>376</v>
       </c>
       <c r="B378" t="n">
-        <v>1445561702.839376</v>
+        <v>795123291.7249727</v>
       </c>
     </row>
     <row r="379">
@@ -3459,7 +3459,7 @@
         <v>377</v>
       </c>
       <c r="B379" t="n">
-        <v>1468484040.404572</v>
+        <v>807729954.8869205</v>
       </c>
     </row>
     <row r="380">
@@ -3467,7 +3467,7 @@
         <v>378</v>
       </c>
       <c r="B380" t="n">
-        <v>1491534612.178619</v>
+        <v>820407475.6638932</v>
       </c>
     </row>
     <row r="381">
@@ -3475,7 +3475,7 @@
         <v>379</v>
       </c>
       <c r="B381" t="n">
-        <v>1514707898.52471</v>
+        <v>833151975.2301202</v>
       </c>
     </row>
     <row r="382">
@@ -3483,7 +3483,7 @@
         <v>380</v>
       </c>
       <c r="B382" t="n">
-        <v>1537998045.590745</v>
+        <v>845961119.7979541</v>
       </c>
     </row>
     <row r="383">
@@ -3491,7 +3491,7 @@
         <v>381</v>
       </c>
       <c r="B383" t="n">
-        <v>1554811347.614815</v>
+        <v>855208011.4171591</v>
       </c>
     </row>
     <row r="384">
@@ -3499,7 +3499,7 @@
         <v>382</v>
       </c>
       <c r="B384" t="n">
-        <v>1571692128.284739</v>
+        <v>864491935.910409</v>
       </c>
     </row>
     <row r="385">
@@ -3507,7 +3507,7 @@
         <v>383</v>
       </c>
       <c r="B385" t="n">
-        <v>1588636031.96566</v>
+        <v>873810145.4572672</v>
       </c>
     </row>
     <row r="386">
@@ -3515,7 +3515,7 @@
         <v>384</v>
       </c>
       <c r="B386" t="n">
-        <v>1605636991.306359</v>
+        <v>883160310.0154107</v>
       </c>
     </row>
     <row r="387">
@@ -3523,7 +3523,7 @@
         <v>385</v>
       </c>
       <c r="B387" t="n">
-        <v>1622690444.289208</v>
+        <v>892539235.8755817</v>
       </c>
     </row>
     <row r="388">
@@ -3531,7 +3531,7 @@
         <v>386</v>
       </c>
       <c r="B388" t="n">
-        <v>1639790873.234804</v>
+        <v>911240286.8779194</v>
       </c>
     </row>
     <row r="389">
@@ -3539,7 +3539,7 @@
         <v>387</v>
       </c>
       <c r="B389" t="n">
-        <v>1656879441.007428</v>
+        <v>929979233.5182416</v>
       </c>
     </row>
     <row r="390">
@@ -3547,7 +3547,7 @@
         <v>388</v>
       </c>
       <c r="B390" t="n">
-        <v>1673377293.397635</v>
+        <v>948424362.0375419</v>
       </c>
     </row>
     <row r="391">
@@ -3555,7 +3555,7 @@
         <v>389</v>
       </c>
       <c r="B391" t="n">
-        <v>1687799094.619394</v>
+        <v>965713524.8190815</v>
       </c>
     </row>
     <row r="392">
@@ -3563,7 +3563,7 @@
         <v>390</v>
       </c>
       <c r="B392" t="n">
-        <v>1698394489.691973</v>
+        <v>980803959.3057193</v>
       </c>
     </row>
     <row r="393">
@@ -3571,7 +3571,7 @@
         <v>391</v>
       </c>
       <c r="B393" t="n">
-        <v>1723086059.783255</v>
+        <v>1012057611.417984</v>
       </c>
     </row>
     <row r="394">
@@ -3579,7 +3579,7 @@
         <v>392</v>
       </c>
       <c r="B394" t="n">
-        <v>1742082021.866847</v>
+        <v>1039733465.564941</v>
       </c>
     </row>
     <row r="395">
@@ -3587,7 +3587,7 @@
         <v>393</v>
       </c>
       <c r="B395" t="n">
-        <v>1755660937.550134</v>
+        <v>1063846317.165733</v>
       </c>
     </row>
     <row r="396">
@@ -3595,7 +3595,7 @@
         <v>394</v>
       </c>
       <c r="B396" t="n">
-        <v>1764630981.510189</v>
+        <v>1084759598.519469</v>
       </c>
     </row>
     <row r="397">
@@ -3603,7 +3603,7 @@
         <v>395</v>
       </c>
       <c r="B397" t="n">
-        <v>1770049701.388512</v>
+        <v>1103032779.821067</v>
       </c>
     </row>
     <row r="398">
@@ -3611,7 +3611,7 @@
         <v>396</v>
       </c>
       <c r="B398" t="n">
-        <v>1773014987.429447</v>
+        <v>1119291514.365979</v>
       </c>
     </row>
     <row r="399">
@@ -3619,7 +3619,7 @@
         <v>397</v>
       </c>
       <c r="B399" t="n">
-        <v>1774531400.710859</v>
+        <v>1134141006.404077</v>
       </c>
     </row>
     <row r="400">
@@ -3627,7 +3627,7 @@
         <v>398</v>
       </c>
       <c r="B400" t="n">
-        <v>1775445855.607762</v>
+        <v>1148117457.648182</v>
       </c>
     </row>
     <row r="401">
@@ -3635,7 +3635,7 @@
         <v>399</v>
       </c>
       <c r="B401" t="n">
-        <v>1776428028.995756</v>
+        <v>1161665617.939994</v>
       </c>
     </row>
     <row r="402">
@@ -3643,7 +3643,7 @@
         <v>400</v>
       </c>
       <c r="B402" t="n">
-        <v>1777976707.031778</v>
+        <v>1175136709.172908</v>
       </c>
     </row>
     <row r="403">
@@ -3651,7 +3651,7 @@
         <v>401</v>
       </c>
       <c r="B403" t="n">
-        <v>1833971289.572975</v>
+        <v>1242324669.348424</v>
       </c>
     </row>
     <row r="404">
@@ -3659,7 +3659,7 @@
         <v>402</v>
       </c>
       <c r="B404" t="n">
-        <v>1888680040.152385</v>
+        <v>1307460206.9105</v>
       </c>
     </row>
     <row r="405">
@@ -3667,7 +3667,7 @@
         <v>403</v>
       </c>
       <c r="B405" t="n">
-        <v>1942408564.249466</v>
+        <v>1370848518.454901</v>
       </c>
     </row>
     <row r="406">
@@ -3675,7 +3675,7 @@
         <v>404</v>
       </c>
       <c r="B406" t="n">
-        <v>1995411704.122757</v>
+        <v>1432767005.274234</v>
       </c>
     </row>
     <row r="407">
@@ -3683,7 +3683,7 @@
         <v>405</v>
       </c>
       <c r="B407" t="n">
-        <v>2047896215.955525</v>
+        <v>1493463985.615654</v>
       </c>
     </row>
     <row r="408">
@@ -3691,7 +3691,7 @@
         <v>406</v>
       </c>
       <c r="B408" t="n">
-        <v>2100027379.125194</v>
+        <v>1553154563.190977</v>
       </c>
     </row>
     <row r="409">
@@ -3699,7 +3699,7 @@
         <v>407</v>
       </c>
       <c r="B409" t="n">
-        <v>2151934727.020473</v>
+        <v>1612024990.107913</v>
       </c>
     </row>
     <row r="410">
@@ -3707,7 +3707,7 @@
         <v>408</v>
       </c>
       <c r="B410" t="n">
-        <v>2203717868.132726</v>
+        <v>1670231909.053203</v>
       </c>
     </row>
     <row r="411">
@@ -3715,7 +3715,7 @@
         <v>409</v>
       </c>
       <c r="B411" t="n">
-        <v>2255451357.50292</v>
+        <v>1727907292.0341</v>
       </c>
     </row>
     <row r="412">
@@ -3723,7 +3723,7 @@
         <v>410</v>
       </c>
       <c r="B412" t="n">
-        <v>2307189739.50681</v>
+        <v>1785160960.894238</v>
       </c>
     </row>
     <row r="413">
@@ -3731,7 +3731,7 @@
         <v>411</v>
       </c>
       <c r="B413" t="n">
-        <v>2334038951.169407</v>
+        <v>1817150606.615945</v>
       </c>
     </row>
     <row r="414">
@@ -3739,7 +3739,7 @@
         <v>412</v>
       </c>
       <c r="B414" t="n">
-        <v>2361328881.139693</v>
+        <v>1849254310.889244</v>
       </c>
     </row>
     <row r="415">
@@ -3747,7 +3747,7 @@
         <v>413</v>
       </c>
       <c r="B415" t="n">
-        <v>2389131467.005021</v>
+        <v>1881589212.428437</v>
       </c>
     </row>
     <row r="416">
@@ -3755,7 +3755,7 @@
         <v>414</v>
       </c>
       <c r="B416" t="n">
-        <v>2417407254.395346</v>
+        <v>1914155105.932707</v>
       </c>
     </row>
     <row r="417">
@@ -3763,7 +3763,7 @@
         <v>415</v>
       </c>
       <c r="B417" t="n">
-        <v>2446116160.784106</v>
+        <v>1946949096.39582</v>
       </c>
     </row>
     <row r="418">
@@ -3771,7 +3771,7 @@
         <v>416</v>
       </c>
       <c r="B418" t="n">
-        <v>2475217986.766279</v>
+        <v>1979963661.231501</v>
       </c>
     </row>
     <row r="419">
@@ -3779,7 +3779,7 @@
         <v>417</v>
       </c>
       <c r="B419" t="n">
-        <v>2504380766.443476</v>
+        <v>2012953662.054559</v>
       </c>
     </row>
     <row r="420">
@@ -3787,7 +3787,7 @@
         <v>418</v>
       </c>
       <c r="B420" t="n">
-        <v>2530311946.729125</v>
+        <v>2043259847.697798</v>
       </c>
     </row>
     <row r="421">
@@ -3795,7 +3795,7 @@
         <v>419</v>
       </c>
       <c r="B421" t="n">
-        <v>2544603888.71852</v>
+        <v>2064006554.018771</v>
       </c>
     </row>
     <row r="422">
@@ -3803,7 +3803,7 @@
         <v>420</v>
       </c>
       <c r="B422" t="n">
-        <v>2537365108.506991</v>
+        <v>2067014022.271347</v>
       </c>
     </row>
     <row r="423">
@@ -3811,7 +3811,7 @@
         <v>421</v>
       </c>
       <c r="B423" t="n">
-        <v>2502012062.029463</v>
+        <v>2046723960.688963</v>
       </c>
     </row>
     <row r="424">
@@ -3819,7 +3819,7 @@
         <v>422</v>
       </c>
       <c r="B424" t="n">
-        <v>2437073211.189877</v>
+        <v>2001735256.256716</v>
       </c>
     </row>
     <row r="425">
@@ -3827,7 +3827,7 @@
         <v>423</v>
       </c>
       <c r="B425" t="n">
-        <v>2345418915.0537</v>
+        <v>1934227306.686744</v>
       </c>
     </row>
     <row r="426">
@@ -3835,7 +3835,7 @@
         <v>424</v>
       </c>
       <c r="B426" t="n">
-        <v>2232519259.345423</v>
+        <v>1848560379.580116</v>
       </c>
     </row>
     <row r="427">
@@ -3843,7 +3843,7 @@
         <v>425</v>
       </c>
       <c r="B427" t="n">
-        <v>2104798971.362617</v>
+        <v>1749936719.400182</v>
       </c>
     </row>
     <row r="428">
@@ -3851,7 +3851,7 @@
         <v>426</v>
       </c>
       <c r="B428" t="n">
-        <v>1968495490.975441</v>
+        <v>1643453007.417205</v>
       </c>
     </row>
     <row r="429">
@@ -3859,7 +3859,7 @@
         <v>427</v>
       </c>
       <c r="B429" t="n">
-        <v>1829017074.474315</v>
+        <v>1533566385.812495</v>
       </c>
     </row>
     <row r="430">
@@ -3867,7 +3867,7 @@
         <v>428</v>
       </c>
       <c r="B430" t="n">
-        <v>1690685801.24449</v>
+        <v>1423868257.204588</v>
       </c>
     </row>
     <row r="431">
@@ -3875,7 +3875,7 @@
         <v>429</v>
       </c>
       <c r="B431" t="n">
-        <v>1556724665.371577</v>
+        <v>1317065899.13135</v>
       </c>
     </row>
     <row r="432">
@@ -3883,7 +3883,7 @@
         <v>430</v>
       </c>
       <c r="B432" t="n">
-        <v>1429367296.066275</v>
+        <v>1215061947.379647</v>
       </c>
     </row>
     <row r="433">
@@ -3891,7 +3891,7 @@
         <v>431</v>
       </c>
       <c r="B433" t="n">
-        <v>1310025229.908217</v>
+        <v>1119088315.351106</v>
       </c>
     </row>
     <row r="434">
@@ -3899,7 +3899,7 @@
         <v>432</v>
       </c>
       <c r="B434" t="n">
-        <v>1199464382.860801</v>
+        <v>1029845504.455908</v>
       </c>
     </row>
     <row r="435">
@@ -3907,7 +3907,7 @@
         <v>433</v>
       </c>
       <c r="B435" t="n">
-        <v>1097961744.556799</v>
+        <v>947628204.1038709</v>
       </c>
     </row>
     <row r="436">
@@ -3915,7 +3915,7 @@
         <v>434</v>
       </c>
       <c r="B436" t="n">
-        <v>1005442795.341471</v>
+        <v>872438172.7330658</v>
       </c>
     </row>
     <row r="437">
@@ -3923,7 +3923,7 @@
         <v>435</v>
       </c>
       <c r="B437" t="n">
-        <v>921595009.3949554</v>
+        <v>804075060.2871873</v>
       </c>
     </row>
     <row r="438">
@@ -3931,7 +3931,7 @@
         <v>436</v>
       </c>
       <c r="B438" t="n">
-        <v>845948868.4646014</v>
+        <v>742202485.3412361</v>
       </c>
     </row>
     <row r="439">
@@ -3939,7 +3939,7 @@
         <v>437</v>
       </c>
       <c r="B439" t="n">
-        <v>777944235.1159639</v>
+        <v>686405468.748835</v>
       </c>
     </row>
     <row r="440">
@@ -3947,7 +3947,7 @@
         <v>438</v>
       </c>
       <c r="B440" t="n">
-        <v>716978813.6702818</v>
+        <v>636225764.793499</v>
       </c>
     </row>
     <row r="441">
@@ -3955,7 +3955,7 @@
         <v>439</v>
       </c>
       <c r="B441" t="n">
-        <v>662439328.2265866</v>
+        <v>591194132.211248</v>
       </c>
     </row>
     <row r="442">
@@ -3963,7 +3963,7 @@
         <v>440</v>
       </c>
       <c r="B442" t="n">
-        <v>613725967.1601751</v>
+        <v>550846245.355486</v>
       </c>
     </row>
     <row r="443">
@@ -3971,7 +3971,7 @@
         <v>441</v>
       </c>
       <c r="B443" t="n">
-        <v>570265354.2269646</v>
+        <v>514733846.3452652</v>
       </c>
     </row>
     <row r="444">
@@ -3979,7 +3979,7 @@
         <v>442</v>
       </c>
       <c r="B444" t="n">
-        <v>531519590.8534323</v>
+        <v>482434797.1793395</v>
       </c>
     </row>
     <row r="445">
@@ -3987,7 +3987,7 @@
         <v>443</v>
       </c>
       <c r="B445" t="n">
-        <v>496994980.4737478</v>
+        <v>453559404.7560069</v>
       </c>
     </row>
     <row r="446">
@@ -3995,7 +3995,7 @@
         <v>444</v>
       </c>
       <c r="B446" t="n">
-        <v>466236723.9006115</v>
+        <v>427750349.0740141</v>
       </c>
     </row>
     <row r="447">
@@ -4003,7 +4003,7 @@
         <v>445</v>
       </c>
       <c r="B447" t="n">
-        <v>438833293.3217613</v>
+        <v>404681221.7211356</v>
       </c>
     </row>
     <row r="448">
@@ -4011,7 +4011,7 @@
         <v>446</v>
       </c>
       <c r="B448" t="n">
-        <v>414414515.7395141</v>
+        <v>384057304.4578423</v>
       </c>
     </row>
     <row r="449">
@@ -4019,7 +4019,7 @@
         <v>447</v>
       </c>
       <c r="B449" t="n">
-        <v>392649513.497398</v>
+        <v>365615261.8214278</v>
       </c>
     </row>
     <row r="450">
@@ -4027,7 +4027,7 @@
         <v>448</v>
       </c>
       <c r="B450" t="n">
-        <v>373241819.6849245</v>
+        <v>349118412.0930201</v>
       </c>
     </row>
     <row r="451">
@@ -4035,7 +4035,7 @@
         <v>449</v>
       </c>
       <c r="B451" t="n">
-        <v>355929678.1018269</v>
+        <v>334355896.6509011</v>
       </c>
     </row>
     <row r="452">

</xml_diff>